<commit_message>
still testing keyword substitution in xlsx and docx files
SVN-Revision: 142
</commit_message>
<xml_diff>
--- a/database/data/substitutionTest.xlsx
+++ b/database/data/substitutionTest.xlsx
@@ -25,7 +25,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$Revision$</t>
+    <t>$Rev$</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -403,7 +403,7 @@
   <dimension ref="B3:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>